<commit_message>
added user stories and updated order
</commit_message>
<xml_diff>
--- a/Product_Backlog/Backlog.xlsx
+++ b/Product_Backlog/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\AC31007-Agile\AC31007-AgileProject\Product_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8AAD7E-00F8-4254-AC69-4F050D4F2E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240B8C80-68B0-41F7-932C-EFF8EB0B1946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8B4862AD-D38D-4800-A3C5-0F2C9B58B532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>get their answers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> be able to export data from a questionnaire as a CSV file</t>
   </si>
   <si>
     <t>analyse it later.</t>
@@ -463,21 +460,59 @@
 • different file format</t>
   </si>
   <si>
-    <t xml:space="preserve">Open answer, 
-multiple choice 
-(1+ possible answers), 
-System Usability Scale https://www.researchgate.net/figure/The-System-Usability-Scale-SUS-questionnaire_fig6_271336759) </t>
-  </si>
-  <si>
     <t>see example file:
 title, description, name, contact, etc.</t>
+  </si>
+  <si>
+    <t>add a multiple choice question</t>
+  </si>
+  <si>
+    <t>add a System Usability Scale</t>
+  </si>
+  <si>
+    <t>how many answer options?</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/figure/The-System-Usability-Scale-SUS-questionnaire_fig6_271336759</t>
+  </si>
+  <si>
+    <t>add an open answer question</t>
+  </si>
+  <si>
+    <t>choose type, 
+choose title and description, 
+mandatory?</t>
+  </si>
+  <si>
+    <t>ask participants to write their own answers.</t>
+  </si>
+  <si>
+    <t>ask participants to select a given answer.</t>
+  </si>
+  <si>
+    <t>ask participants to rate different statements.</t>
+  </si>
+  <si>
+    <t>• enter any characters
+• text length?</t>
+  </si>
+  <si>
+    <t>• add new answer option
+• remove/ edit answer</t>
+  </si>
+  <si>
+    <t>• edit answer range
+• add new statement</t>
+  </si>
+  <si>
+    <t>be able to export data from a questionnaire as a CSV file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +554,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -661,10 +704,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,8 +787,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -767,45 +818,12 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="-1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -833,10 +851,45 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -886,39 +939,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -970,15 +990,15 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1006,11 +1026,42 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="-1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1215,20 +1266,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K38" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K38" xr:uid="{6BD4E4A1-15EF-43F4-A1F0-6FEB3AABF1FF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K41" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K41" xr:uid="{6BD4E4A1-15EF-43F4-A1F0-6FEB3AABF1FF}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{8F9B6BFC-5AC2-408E-9C5F-D1EF4B858B00}" name="ID" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{BB1D8BD0-D244-40D2-A502-2AE8DA2533EE}" name="As a &lt; type of user &gt;" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{45D566F8-9B7E-4186-BBF3-AECBFE3AC7AC}" name="I want to &lt; perform some task &gt;" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="4"/>
     <tableColumn id="10" xr3:uid="{FC079366-522B-4852-AD58-E43650253517}" name="Test Proposition" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1534,7 +1585,7 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -1543,11 +1594,12 @@
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="17.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="32" style="3" customWidth="1"/>
-    <col min="4" max="5" width="26.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="17" customWidth="1"/>
     <col min="8" max="8" width="49.28515625" style="24" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="19"/>
@@ -1558,13 +1610,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -1573,16 +1625,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>3</v>
@@ -1599,19 +1651,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="I2" s="6">
         <v>5</v>
@@ -1620,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1631,22 +1683,22 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I3" s="5">
         <v>3</v>
@@ -1655,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1672,16 +1724,16 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I4" s="6">
         <v>5</v>
@@ -1690,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1698,23 +1750,23 @@
         <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I5" s="6">
         <v>3</v>
@@ -1723,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1731,23 +1783,23 @@
         <v>25</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="6">
         <v>2</v>
@@ -1756,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1767,20 +1819,20 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" s="6">
         <v>2</v>
@@ -1789,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1806,273 +1858,267 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I8" s="6">
         <v>5</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>34</v>
-      </c>
+      <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>95</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5</v>
+        <v>129</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>7</v>
-      </c>
+      <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>95</v>
-      </c>
+      <c r="C10" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" s="6">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>5</v>
-      </c>
+      <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="6">
-        <v>5</v>
+      <c r="C11" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="6" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="22"/>
+        <v>94</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>111</v>
+      </c>
       <c r="I12" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="6" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="22"/>
+        <v>94</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="I13" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="6">
-        <v>2</v>
+      <c r="H15" s="27"/>
+      <c r="I15" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>95</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="6" t="s">
@@ -2087,262 +2133,260 @@
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>38</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="A18" s="5">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>95</v>
       </c>
       <c r="H18" s="22"/>
-      <c r="I18" s="8">
-        <v>8</v>
-      </c>
-      <c r="J18" s="18"/>
+      <c r="I18" s="6">
+        <v>3</v>
+      </c>
+      <c r="J18" s="14"/>
       <c r="K18" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>42</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="5" t="s">
-        <v>99</v>
+        <v>27</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="6">
+        <v>3</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H24" s="22"/>
-      <c r="I24" s="6" t="s">
-        <v>99</v>
+      <c r="I24" s="6">
+        <v>2</v>
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>96</v>
+      <c r="A25" s="7">
+        <v>38</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="H25" s="22"/>
-      <c r="I25" s="6">
+      <c r="I25" s="8">
         <v>8</v>
       </c>
-      <c r="J25" s="14"/>
+      <c r="J25" s="18"/>
       <c r="K25" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="6">
@@ -2350,117 +2394,115 @@
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H27" s="22"/>
-      <c r="I27" s="6">
-        <v>3</v>
+      <c r="I27" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="6" t="s">
         <v>86</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>36</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="6">
@@ -2468,206 +2510,204 @@
       </c>
       <c r="J30" s="14"/>
       <c r="K30" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F32" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H33" s="22"/>
-      <c r="I33" s="6" t="s">
-        <v>99</v>
+      <c r="I33" s="6">
+        <v>3</v>
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H35" s="22"/>
-      <c r="I35" s="6" t="s">
-        <v>99</v>
+      <c r="I35" s="6">
+        <v>5</v>
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>92</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E37" s="9"/>
       <c r="F37" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="6">
@@ -2675,47 +2715,141 @@
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H38" s="22"/>
-      <c r="I38" s="6">
-        <v>8</v>
+      <c r="I38" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D64" s="11"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>11</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J39" s="14"/>
+      <c r="K39" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>20</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="6">
+        <v>8</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="K40" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>6</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="6">
+        <v>8</v>
+      </c>
+      <c r="J41" s="14"/>
+      <c r="K41" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{C5112DD5-35C8-4F9E-8A3D-EB2708C0916D}"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated product backlog for sprint review
</commit_message>
<xml_diff>
--- a/Product_Backlog/Backlog.xlsx
+++ b/Product_Backlog/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\AC31007-Agile\AC31007-AgileProject\Product_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240B8C80-68B0-41F7-932C-EFF8EB0B1946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7746840-18EA-41CA-A74E-E931E1EDD81A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8B4862AD-D38D-4800-A3C5-0F2C9B58B532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="134">
   <si>
     <t>ID</t>
   </si>
@@ -204,22 +204,7 @@
     <t>fully analyse them.</t>
   </si>
   <si>
-    <t xml:space="preserve">have a list of all my Co-researchers </t>
-  </si>
-  <si>
-    <t>select different people for different parts of the project.</t>
-  </si>
-  <si>
-    <t>select the experiments each of my CoRs has access to</t>
-  </si>
-  <si>
-    <t>restrict their access to approved experiments.</t>
-  </si>
-  <si>
     <t>Co-Researcher</t>
-  </si>
-  <si>
-    <t>have only access to parts my PR has selected</t>
   </si>
   <si>
     <t>ensure the protection of sensible data.</t>
@@ -470,42 +455,60 @@
     <t>add a System Usability Scale</t>
   </si>
   <si>
-    <t>how many answer options?</t>
-  </si>
-  <si>
     <t>https://www.researchgate.net/figure/The-System-Usability-Scale-SUS-questionnaire_fig6_271336759</t>
   </si>
   <si>
     <t>add an open answer question</t>
+  </si>
+  <si>
+    <t>ask participants to write their own answers.</t>
+  </si>
+  <si>
+    <t>ask participants to select a given answer.</t>
+  </si>
+  <si>
+    <t>ask participants to rate different statements.</t>
+  </si>
+  <si>
+    <t>• enter any characters
+• text length?</t>
+  </si>
+  <si>
+    <t>• add new answer option
+• remove/ edit answer</t>
+  </si>
+  <si>
+    <t>• edit answer range
+• add new statement</t>
+  </si>
+  <si>
+    <t>be able to export data from a questionnaire as a CSV file</t>
+  </si>
+  <si>
+    <t>add new co-researchers to my experiments</t>
+  </si>
+  <si>
+    <t>delete excisting co-researchers from my experiments</t>
+  </si>
+  <si>
+    <t>collaborate with other scientists.</t>
+  </si>
+  <si>
+    <t>restrict access to my research.</t>
+  </si>
+  <si>
+    <t>have access to experiments assigned to me by a PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Researcher </t>
   </si>
   <si>
     <t>choose type, 
 choose title and description, 
-mandatory?</t>
-  </si>
-  <si>
-    <t>ask participants to write their own answers.</t>
-  </si>
-  <si>
-    <t>ask participants to select a given answer.</t>
-  </si>
-  <si>
-    <t>ask participants to rate different statements.</t>
-  </si>
-  <si>
-    <t>• enter any characters
-• text length?</t>
-  </si>
-  <si>
-    <t>• add new answer option
-• remove/ edit answer</t>
-  </si>
-  <si>
-    <t>• edit answer range
-• add new statement</t>
-  </si>
-  <si>
-    <t>be able to export data from a questionnaire as a CSV file</t>
+choose if answer mandatory</t>
+  </si>
+  <si>
+    <t>add answer options</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,12 +796,49 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1266,20 +1306,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K41" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:K41" xr:uid="{6BD4E4A1-15EF-43F4-A1F0-6FEB3AABF1FF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8F9B6BFC-5AC2-408E-9C5F-D1EF4B858B00}" name="ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{BB1D8BD0-D244-40D2-A502-2AE8DA2533EE}" name="As a &lt; type of user &gt;" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{45D566F8-9B7E-4186-BBF3-AECBFE3AC7AC}" name="I want to &lt; perform some task &gt;" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{FC079366-522B-4852-AD58-E43650253517}" name="Test Proposition" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8F9B6BFC-5AC2-408E-9C5F-D1EF4B858B00}" name="ID" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{BB1D8BD0-D244-40D2-A502-2AE8DA2533EE}" name="As a &lt; type of user &gt;" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{45D566F8-9B7E-4186-BBF3-AECBFE3AC7AC}" name="I want to &lt; perform some task &gt;" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{FC079366-522B-4852-AD58-E43650253517}" name="Test Proposition" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1587,8 +1627,8 @@
   </sheetPr>
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1642,8 @@
     <col min="7" max="7" width="9.85546875" style="17" customWidth="1"/>
     <col min="8" max="8" width="49.28515625" style="24" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="19"/>
+    <col min="10" max="10" width="9.140625" style="19"/>
+    <col min="11" max="11" width="11" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1610,13 +1651,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -1625,16 +1666,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K1" s="20" t="s">
         <v>3</v>
@@ -1651,19 +1692,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I2" s="6">
         <v>5</v>
@@ -1672,33 +1713,33 @@
         <v>1</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>39</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I3" s="5">
         <v>3</v>
@@ -1706,8 +1747,8 @@
       <c r="J3" s="14">
         <v>1</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>100</v>
+      <c r="K3" s="31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,16 +1765,16 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I4" s="6">
         <v>5</v>
@@ -1742,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1750,23 +1791,23 @@
         <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I5" s="6">
         <v>3</v>
@@ -1775,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,13 +1834,13 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I6" s="6">
         <v>2</v>
@@ -1808,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1826,13 +1867,13 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I7" s="6">
         <v>2</v>
@@ -1841,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1858,23 +1899,23 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I8" s="6">
         <v>5</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1883,23 +1924,23 @@
         <v>6</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="5"/>
       <c r="G9" s="14"/>
       <c r="H9" s="22" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,25 +1949,25 @@
         <v>6</v>
       </c>
       <c r="C10" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>127</v>
-      </c>
       <c r="E10" s="26" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="14"/>
       <c r="H10" s="22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,25 +1976,25 @@
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>128</v>
-      </c>
       <c r="E11" s="29" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="14"/>
       <c r="H11" s="22" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1961,150 +2002,150 @@
         <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I12" s="6">
         <v>5</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="6" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>118</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H13" s="22"/>
       <c r="I13" s="6">
         <v>5</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="6">
-        <v>5</v>
+      <c r="C14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>42</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="5" t="s">
-        <v>98</v>
+      <c r="C15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="6">
+        <v>5</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="6" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" s="22"/>
+        <v>89</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="I16" s="6">
         <v>5</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,10 +2163,10 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="6">
@@ -2133,7 +2174,7 @@
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2151,10 +2192,10 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="6">
@@ -2162,7 +2203,7 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2170,20 +2211,20 @@
         <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="6">
@@ -2191,86 +2232,66 @@
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>26</v>
-      </c>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="6">
-        <v>2</v>
-      </c>
+      <c r="C20" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>27</v>
-      </c>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="6">
-        <v>3</v>
-      </c>
+      <c r="C21" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="25" t="s">
-        <v>106</v>
-      </c>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="6">
@@ -2278,28 +2299,28 @@
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="6">
@@ -2307,28 +2328,28 @@
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="6">
@@ -2336,7 +2357,7 @@
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2344,20 +2365,20 @@
         <v>38</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="8">
@@ -2365,7 +2386,7 @@
       </c>
       <c r="J25" s="18"/>
       <c r="K25" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,10 +2404,10 @@
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="6">
@@ -2394,7 +2415,7 @@
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2402,7 +2423,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>42</v>
@@ -2412,18 +2433,18 @@
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,7 +2452,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>4</v>
@@ -2441,10 +2462,10 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="6">
@@ -2452,7 +2473,7 @@
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2470,10 +2491,10 @@
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="6">
@@ -2481,7 +2502,7 @@
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2489,20 +2510,20 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="6">
@@ -2510,7 +2531,7 @@
       </c>
       <c r="J30" s="14"/>
       <c r="K30" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2518,7 +2539,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>18</v>
@@ -2528,10 +2549,10 @@
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="6">
@@ -2539,7 +2560,7 @@
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2559,10 +2580,10 @@
         <v>35</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="6">
@@ -2570,7 +2591,7 @@
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,10 +2609,10 @@
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="6">
@@ -2599,7 +2620,7 @@
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2617,10 +2638,10 @@
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="6">
@@ -2628,7 +2649,7 @@
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,10 +2667,10 @@
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="6">
@@ -2657,7 +2678,7 @@
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2675,18 +2696,18 @@
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2697,17 +2718,17 @@
         <v>6</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="6">
@@ -2715,7 +2736,7 @@
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2733,18 +2754,18 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2752,7 +2773,7 @@
         <v>11</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>24</v>
@@ -2764,18 +2785,18 @@
         <v>26</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J39" s="14"/>
       <c r="K39" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2792,13 +2813,13 @@
         <v>45</v>
       </c>
       <c r="E40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="6">
@@ -2806,7 +2827,7 @@
       </c>
       <c r="J40" s="14"/>
       <c r="K40" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2824,10 +2845,10 @@
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="6">
@@ -2835,7 +2856,7 @@
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2843,6 +2864,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="To be Started">
+      <formula>NOT(ISERROR(SEARCH("To be Started",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1" xr:uid="{C5112DD5-35C8-4F9E-8A3D-EB2708C0916D}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
update after end of sprint 1
</commit_message>
<xml_diff>
--- a/Product_Backlog/Backlog.xlsx
+++ b/Product_Backlog/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\AC31007-Agile\AC31007-AgileProject\Product_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7746840-18EA-41CA-A74E-E931E1EDD81A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165562E9-7BFF-4A01-85BD-69CE1C780A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8B4862AD-D38D-4800-A3C5-0F2C9B58B532}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{8B4862AD-D38D-4800-A3C5-0F2C9B58B532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
   <si>
     <t>ID</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Test Proposition</t>
   </si>
   <si>
@@ -510,12 +507,63 @@
   <si>
     <t>add answer options</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• rejected if 1+ fields empty
+• check if properly added to database </t>
+  </si>
+  <si>
+    <t>inform participants about associated aspects.</t>
+  </si>
+  <si>
+    <t>add general information to a questionnaire</t>
+  </si>
+  <si>
+    <t>access to my own experiments erime: squestionnaire, video  eulscrips, n ctrssny, esc.</t>
+  </si>
+  <si>
+    <t>be abinue if box checked
+• compare before s</t>
+  </si>
+  <si>
+    <t>know t as wns, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>see th as we1s, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>2 cta sesurcteonents a. 2 ents  cta sesurcteon acao-.</t>
+  </si>
+  <si>
+    <t>be abl as me1s, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>analys : Reseai mn1i, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>carry  : Reseai wai, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>take n as ma2s, 
+max 125MB</t>
+  </si>
+  <si>
+    <t>have a Mab wa3b, 
+max 125MB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,8 +614,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,6 +638,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,7 +772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -799,16 +860,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -841,6 +916,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1306,20 +1391,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K41" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:K41" xr:uid="{6BD4E4A1-15EF-43F4-A1F0-6FEB3AABF1FF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB590F06-CBDE-428B-8D35-9DA0A5119B65}" name="Table2" displayName="Table2" ref="A1:K42" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:K42" xr:uid="{6BD4E4A1-15EF-43F4-A1F0-6FEB3AABF1FF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8F9B6BFC-5AC2-408E-9C5F-D1EF4B858B00}" name="ID" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{BB1D8BD0-D244-40D2-A502-2AE8DA2533EE}" name="As a &lt; type of user &gt;" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{45D566F8-9B7E-4186-BBF3-AECBFE3AC7AC}" name="I want to &lt; perform some task &gt;" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{FC079366-522B-4852-AD58-E43650253517}" name="Test Proposition" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{8F9B6BFC-5AC2-408E-9C5F-D1EF4B858B00}" name="ID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{BB1D8BD0-D244-40D2-A502-2AE8DA2533EE}" name="As a &lt; type of user &gt;" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{45D566F8-9B7E-4186-BBF3-AECBFE3AC7AC}" name="I want to &lt; perform some task &gt;" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{6EB93109-A1A1-42AA-8DF6-774AA2673987}" name="so that I can &lt; achieve some goal &gt;" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{ABB0FD00-31E1-49E6-826D-3D4AEB69A283}" name="Comment" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{EFBABB0E-4C2C-4990-81E9-4B1B7B74F2F5}" name="Priority" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{E17E2082-183B-405D-BE65-6D6D8370BB2F}" name="MoSCoW" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{FC079366-522B-4852-AD58-E43650253517}" name="Test Proposition" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{1B0E1245-C8BE-419A-B6F1-21D856ECBC79}" name="Story Points" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{676BAE5F-F932-4086-B615-9A0E83C2AA3C}" name="Sprint" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{56FED7EA-F6F9-4FAE-9995-BE081205365E}" name="Status" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1625,10 +1710,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1754,7 @@
         <v>88</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>85</v>
@@ -1692,10 +1777,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>79</v>
@@ -1704,7 +1789,7 @@
         <v>89</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I2" s="6">
         <v>5</v>
@@ -1713,15 +1798,15 @@
         <v>1</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>39</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>83</v>
@@ -1730,7 +1815,7 @@
         <v>84</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
@@ -1739,7 +1824,7 @@
         <v>89</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="5">
         <v>3</v>
@@ -1747,8 +1832,8 @@
       <c r="J3" s="14">
         <v>1</v>
       </c>
-      <c r="K3" s="31" t="s">
-        <v>95</v>
+      <c r="K3" s="21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,9 +1849,7 @@
       <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>114</v>
-      </c>
+      <c r="E4" s="9"/>
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1774,7 +1857,7 @@
         <v>89</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="6">
         <v>5</v>
@@ -1783,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,7 +1890,7 @@
         <v>89</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="6">
         <v>3</v>
@@ -1816,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,7 +1915,9 @@
       <c r="D6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>137</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>79</v>
       </c>
@@ -1840,7 +1925,7 @@
         <v>89</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="6">
         <v>2</v>
@@ -1849,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,7 +1950,9 @@
       <c r="D7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>79</v>
       </c>
@@ -1873,7 +1960,7 @@
         <v>89</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="6">
         <v>2</v>
@@ -1882,286 +1969,302 @@
         <v>1</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
+        <v>79</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I8" s="6">
-        <v>5</v>
-      </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="14"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="H9" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
       </c>
       <c r="J9" s="14"/>
-      <c r="K9" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="K9" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>80</v>
+      </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>133</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E10" s="28"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="H10" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>93</v>
       </c>
       <c r="J10" s="14"/>
-      <c r="K10" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="K10" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>81</v>
+      </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>132</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="H11" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>93</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="K11" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
         <v>89</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" s="6">
-        <v>5</v>
+        <v>123</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="J12" s="14"/>
-      <c r="K12" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="6" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="I13" s="6">
         <v>5</v>
       </c>
       <c r="J13" s="14"/>
-      <c r="K13" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>42</v>
-      </c>
-      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="5" t="s">
-        <v>93</v>
+      <c r="C14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="6">
+        <v>5</v>
       </c>
       <c r="J14" s="14"/>
-      <c r="K14" s="25" t="s">
-        <v>101</v>
+      <c r="K14" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="6" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="22"/>
+        <v>89</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>112</v>
+      </c>
       <c r="I15" s="6">
         <v>5</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>139</v>
+      </c>
       <c r="F16" s="6" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>113</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H16" s="22"/>
       <c r="I16" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="F17" s="6" t="s">
         <v>81</v>
       </c>
@@ -2170,32 +2273,32 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="6">
@@ -2203,40 +2306,40 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="6">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>84</v>
+      </c>
       <c r="B20" s="6" t="s">
         <v>53</v>
       </c>
@@ -2248,72 +2351,90 @@
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" s="32" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="K20" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>28</v>
+      </c>
       <c r="B21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="5"/>
+      <c r="D21" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="6">
+        <v>2</v>
+      </c>
       <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>89</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="6" t="s">
@@ -2324,85 +2445,89 @@
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>33</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="6" t="s">
+      <c r="A24" s="7">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="8">
+        <v>8</v>
+      </c>
+      <c r="J24" s="18"/>
+      <c r="K24" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>42</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="6">
-        <v>2</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>38</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="8">
-        <v>8</v>
-      </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="31" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="F26" s="6" t="s">
         <v>80</v>
       </c>
@@ -2414,24 +2539,26 @@
         <v>5</v>
       </c>
       <c r="J26" s="14"/>
-      <c r="K26" s="25" t="s">
-        <v>101</v>
+      <c r="K26" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="F27" s="6" t="s">
         <v>80</v>
       </c>
@@ -2439,175 +2566,183 @@
         <v>90</v>
       </c>
       <c r="H27" s="22"/>
-      <c r="I27" s="6" t="s">
-        <v>93</v>
+      <c r="I27" s="6">
+        <v>5</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="F28" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>90</v>
       </c>
       <c r="H28" s="22"/>
-      <c r="I28" s="6">
-        <v>8</v>
+      <c r="I28" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="F29" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>90</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J29" s="14"/>
       <c r="K29" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="F30" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>90</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J30" s="14"/>
       <c r="K30" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="F31" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="6">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F33" s="6" t="s">
         <v>82</v>
       </c>
@@ -2620,21 +2755,21 @@
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="6" t="s">
@@ -2649,21 +2784,21 @@
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
@@ -2674,25 +2809,25 @@
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="6" t="s">
@@ -2702,93 +2837,91 @@
         <v>91</v>
       </c>
       <c r="H36" s="22"/>
-      <c r="I36" s="6" t="s">
-        <v>93</v>
+      <c r="I36" s="6">
+        <v>5</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H37" s="22"/>
-      <c r="I37" s="6">
-        <v>8</v>
+      <c r="I37" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H38" s="22"/>
-      <c r="I38" s="6" t="s">
-        <v>93</v>
+      <c r="I38" s="6">
+        <v>8</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E39" s="9"/>
       <c r="F39" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="6" t="s">
@@ -2796,56 +2929,58 @@
       </c>
       <c r="J39" s="14"/>
       <c r="K39" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H40" s="22"/>
-      <c r="I40" s="6">
-        <v>8</v>
+      <c r="I40" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="J40" s="14"/>
       <c r="K40" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="F41" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>91</v>
@@ -2856,24 +2991,58 @@
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="11"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>6</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="6">
+        <v>8</v>
+      </c>
+      <c r="J42" s="14"/>
+      <c r="K42" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="To be Started">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="To be Started">
       <formula>NOT(ISERROR(SEARCH("To be Started",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K7">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{C5112DD5-35C8-4F9E-8A3D-EB2708C0916D}"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{C5112DD5-35C8-4F9E-8A3D-EB2708C0916D}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>